<commit_message>
Folder of first 2 links added
</commit_message>
<xml_diff>
--- a/Dataset Links(Filtered-Unfiltered).xlsx
+++ b/Dataset Links(Filtered-Unfiltered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\datasets\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C161A93-FC80-4110-ABFF-C3ADD7FBAE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1137C35-52E6-4DFE-9473-830959A26851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,12 +126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,7 +450,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +490,7 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">

</xml_diff>